<commit_message>
well known dessert stores: add visiting stores
</commit_message>
<xml_diff>
--- a/甜品知名品牌.xlsx
+++ b/甜品知名品牌.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyeu\leagyun\notes\acheulean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leagy\gyrogit\acheulean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FB8E09-B76B-40EE-8155-B4205E03B82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A9D630-5551-4E75-92A0-F8E7F3F3EEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="3888" windowWidth="17220" windowHeight="18792" xr2:uid="{597E4B12-3009-4D1D-853A-7E339F6292A7}"/>
+    <workbookView xWindow="2265" yWindow="1095" windowWidth="11460" windowHeight="9225" activeTab="2" xr2:uid="{597E4B12-3009-4D1D-853A-7E339F6292A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="3" r:id="rId1"/>
+    <sheet name="逛店_商圈覆盖" sheetId="5" r:id="rId2"/>
+    <sheet name="逛店个别店铺" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Brand</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,6 +133,505 @@
   </si>
   <si>
     <t>Originated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>淮海路</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>静安</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>徐汇</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>陆家嘴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前滩</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>新天地</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IAPM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>久光</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>恒隆</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>兴业太古</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>港汇</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>国金</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前滩太古</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大宁久光</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>外滩</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pierre Marcolini</t>
+  </si>
+  <si>
+    <t>Lady M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L'Éclair de Génie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Joël Robuchon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luneurs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pain Chaud</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tiffany Blue Box Café</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cafe Dior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jardin D'Hiver by Boucheron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>La Parisienne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cheesecake Factory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>愚园路</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>La Boulangerie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>建国路</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma Tatin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交通大学</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>静安嘉里中心</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前滩太古里</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>华山路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>幸福里</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>乌鲁木齐路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>胶州路</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>建国西路</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前滩太古里</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前滩太古里</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>滨江</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>/BFC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>外滩</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -138,7 +639,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +668,64 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91DCE8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7CEE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1E6DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2E7CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4EADF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,7 +742,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -201,6 +753,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,18 +1089,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C44E95-E87C-479E-AD11-1FA0DD3E0540}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -541,7 +1111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -552,7 +1122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -563,7 +1133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -574,7 +1144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -585,7 +1155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -596,7 +1166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,7 +1177,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -618,7 +1188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -629,7 +1199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,7 +1210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -656,4 +1226,478 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB93CE38-19EC-40D8-B775-AC644F35F183}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <f>SUM(B4:M4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ref="N5:N15" si="0">SUM(B5:M5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" ref="B16:J16" si="1">SUM(B4:B15)</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <f>SUM(K4:K15)</f>
+        <v>6</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16:M16" si="2">SUM(L4:L15)</f>
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3639930-DC04-49B4-8EF0-4AD8E12FABBE}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
well known dessert stores: add description of feeling
</commit_message>
<xml_diff>
--- a/甜品知名品牌.xlsx
+++ b/甜品知名品牌.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyeu\leagyun\notes\acheulean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leagy\gyrogit\acheulean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB701D3-C813-4362-ACE6-1D1F0A92E505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0143FFE-B9BA-4A94-AB67-4741A9A5DC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15396" yWindow="6624" windowWidth="17220" windowHeight="16800" xr2:uid="{597E4B12-3009-4D1D-853A-7E339F6292A7}"/>
+    <workbookView xWindow="13680" yWindow="240" windowWidth="19065" windowHeight="11295" xr2:uid="{597E4B12-3009-4D1D-853A-7E339F6292A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="个别店铺" sheetId="6" r:id="rId3"/>
     <sheet name="Misc" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="162">
   <si>
     <t>Brand</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,27 +56,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.fauchon.com/</t>
-  </si>
-  <si>
-    <t>https://www.leclairdegenieshop.com/</t>
-  </si>
-  <si>
-    <t>https://www.carlmarletti.com/</t>
-  </si>
-  <si>
-    <t>https://barpompi.it/</t>
-  </si>
-  <si>
-    <t>https://www.lesouffle.fr/english/</t>
-  </si>
-  <si>
-    <t>https://www.paullafayet.com/</t>
-  </si>
-  <si>
-    <t>https://www.pasticceriacova.com/</t>
-  </si>
-  <si>
     <t>https://www.dorchestercollection.com/en</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,9 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://blackstarpastry.foodstorm.com/</t>
-  </si>
-  <si>
     <t>Fauchon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -636,12 +612,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.laduree.fr/</t>
-  </si>
-  <si>
-    <t>https://www.cyrillignac.com/</t>
-  </si>
-  <si>
     <t>Laduree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -650,23 +620,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.christophemichalak.com/</t>
-  </si>
-  <si>
     <t>Michalak</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.pierreherme.com/</t>
-  </si>
-  <si>
     <t>Pierre Herme</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://philippeconticini.fr/</t>
-  </si>
-  <si>
     <t>Philippe Conticini</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -683,14 +644,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.carraras.com/desserts</t>
-  </si>
-  <si>
     <t>https://maison-caffet.com/</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.starbucksreserve.com/en-us</t>
   </si>
   <si>
     <t>Seattle</t>
@@ -1153,13 +1108,237 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>https://www.fauchon.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客观描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.leclairdegenieshop.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配色亮丽浓重, 线条粗犷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carl Marletti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.carlmarletti.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品可爱图形碎花, 放置轻松随意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小姑娘抹口红穿大人衣服, 内心小可爱却想要体验成熟的魅力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>店铺历史感大地色, 店员西装笔挺, 产品包装简约色彩单一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老派贵族二代, 沉稳不守旧, 时尚不先锋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://barpompi.it/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.lesouffle.fr/english/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活在魔法童话里面的上一代少女, 现在是妈妈或外婆了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老旧的配色, 大花字+魔法皇冠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tiffany蓝+比安徒生童话都老的丘比特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.pasticceriacova.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主观感受</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斜体+经典蓝色衬体字体+弧形字造型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>穿上韩式蓝色呢绒大衣的乡村气质女士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大家族出身的优雅亲和的大姐姐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时尚度很高的名媛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瘦衬体, 古堡+皇家/贵族感, 色系偏正</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>细瘦字体, 徽章系统, 淡雅色, 时尚大牌翅膀女模</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>端庄, 仪式感拉满, 小心翼翼又有主见的教养贵族</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blackstarpastry.foodstorm.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆头圆脑的大黑粗体字, 幼稚童趣画风的游戏感</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.paullafayet.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粉红粉蓝配色, 卡通线条图案, 块状组合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粉嘟嘟爱幻想的少女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.laduree.fr/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脏粉+灰紫+亚红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.cyrillignac.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果说Paul Lafayet是13岁, 那这个就是16岁, 开始自我意识的萌芽和恋爱的季节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精致具有主厨感的产品, 不花哨有气质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造诣深厚不妥协的独立思想的主厨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浓妆艳抹的强势御姐, 混迹酒吧夜店, instagram热度博主</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.christophemichalak.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.pierreherme.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风趣乐观轻松阳光随性的大男孩/女孩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5%衬体+95%非衬体, 色系丰富又精致的产品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时尚度拉满的新晋时尚博主, 年轻人的当红话语权</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全是花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://philippeconticini.fr/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当代的洛可可女士, 明亮可爱浪漫华丽满面春风</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淡雅的大地色, 柔和端庄的字体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.carraras.com/desserts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.starbucksreserve.com/en-us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知书达理钢琴十级无敌优雅的长裙姐姐, 阳光照在姐姐一半的脸上, 笑容那么治愈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品色彩纷乱 野性 不修边幅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西部世界的下午茶, 疲惫不堪的牛仔骑着马到小酒馆喝上一杯顺便点个蛋糕给女士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模具中的蛋糕, 手工感一般, 艺术感较低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生意人填饱肚子的伙食, 忙碌生活的一丝惬意, 生活的点缀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巧克力色+金色, 马卡龙颜色暗沉, 老家具感</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住在几百年前灯光昏暗的豪宅中的古板老头子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字间距很宽, 利落的非衬体, 深咖色+光影</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老练活力满满富有创造力的谷歌式白领</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1229,6 +1408,37 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑 Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1277,12 +1487,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1292,13 +1505,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1313,15 +1529,43 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1633,290 +1877,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C44E95-E87C-479E-AD11-1FA0DD3E0540}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="36.375" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.75" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="35.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="58.375" customWidth="1"/>
+    <col min="7" max="7" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
+      <c r="B11" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="B20" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="E20" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E21" s="16"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E22" s="16"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E23" s="16"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{895D3A21-0F32-44F9-80D4-A714583A5147}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{75B60D56-99B0-40B0-89A4-CBAE5FAD4A8F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{5E3870DD-B666-456D-962D-4A6001B2DCBA}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{6A6496C2-4333-4EF3-A05C-D1462A8813B6}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{9C7EC405-3469-4F62-8890-93A5CE4715E2}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{1B3C1659-CB74-40BB-9961-A9E7AA297448}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{64D51139-011D-476B-B242-CCCA7DC68CD6}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{BBD873A4-826E-417F-A765-C90D2D387C09}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{A0AC372F-4631-498F-8F1B-159B8DF0ED0A}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{9C1D1E07-0CFA-4AA0-8212-D2F3CF96119B}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{F6103E17-2AAF-43FB-9AEE-5997A95A338D}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{147E0391-071B-48D2-9BC0-2E5F087837CD}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{4BCC7F7F-0A59-4DC9-A927-64BFD32F6542}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{332A3A20-442A-4B36-8DBB-0780D6E5C239}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{804CD898-8C00-4F1C-845C-ACEE5E3E8C55}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{1A44A26A-F5EF-4D92-84AF-1EEE6B940DEB}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{0A33E7D6-2EC4-4ECB-B37D-F62DA9677535}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{246635F5-05FD-4036-8CA1-67B5E899CB84}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{6CAA4529-AE0E-4435-8986-1E2C84AFBBEC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1928,95 +2393,95 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="26.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="3" spans="1:14" ht="12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -2032,9 +2497,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -2059,7 +2524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2083,9 +2548,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -2095,9 +2560,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -2110,9 +2575,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -2122,9 +2587,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2137,9 +2602,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -2149,9 +2614,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -2161,9 +2626,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -2173,9 +2638,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K14" s="1">
         <v>1</v>
@@ -2185,9 +2650,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -2200,9 +2665,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ref="B16:J16" si="1">SUM(B4:B15)</f>
@@ -2274,117 +2739,117 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -2399,117 +2864,117 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:A21"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>114</v>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>